<commit_message>
Configuration Item List 1.2
</commit_message>
<xml_diff>
--- a/ConfigurationItemList.xlsx
+++ b/ConfigurationItemList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Configuration Item</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Definition of use cases</t>
   </si>
   <si>
-    <t>This Document (Section 2.2)</t>
-  </si>
-  <si>
     <t>Definition of fields</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Configuration Item List</t>
   </si>
   <si>
-    <t>ConfigurationItemList.xlsx</t>
-  </si>
-  <si>
     <t>https://github.com/sungori/SoftBugOff/blob/master/UserRoles.xlsx</t>
   </si>
   <si>
@@ -112,6 +106,15 @@
   </si>
   <si>
     <t>Term Project Document</t>
+  </si>
+  <si>
+    <t>https://github.com/sungori/SoftBugOff/blob/master/ConfigurationItemList.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/sungori/SoftBugOff/blob/master/Giles_Vernon_TermProject.docx</t>
+  </si>
+  <si>
+    <t>https://github.com/sungori/SoftBugOff/blob/master/UseCases.xlsx</t>
   </si>
 </sst>
 </file>
@@ -536,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -585,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1">
@@ -605,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30.75" thickBot="1">
@@ -625,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" thickBot="1">
@@ -645,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" thickBot="1">
@@ -665,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30.75" thickBot="1">
@@ -685,10 +688,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75" thickBot="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -696,16 +699,16 @@
         <v>13</v>
       </c>
       <c r="C8" s="7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="6">
-        <v>41921</v>
+        <v>41928</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
+      <c r="F8" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30.75" thickBot="1">
@@ -713,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
@@ -725,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1">
@@ -733,7 +736,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7">
         <v>0.1</v>
@@ -753,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="7">
         <v>0.1</v>
@@ -773,7 +776,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="7">
         <v>0.1</v>
@@ -785,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1">
@@ -793,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7">
         <v>0.1</v>
@@ -808,15 +811,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+    <row r="14" spans="1:6" ht="30.75" thickBot="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D14" s="6">
         <v>41928</v>
@@ -824,26 +827,28 @@
       <c r="E14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+      <c r="F14" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30.75" thickBot="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="7">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="D15" s="6">
-        <v>41927</v>
+        <v>41928</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
+      <c r="F15" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -855,8 +860,11 @@
     <hyperlink ref="F6" r:id="rId5"/>
     <hyperlink ref="F9" r:id="rId6"/>
     <hyperlink ref="F5" r:id="rId7"/>
+    <hyperlink ref="F15" r:id="rId8"/>
+    <hyperlink ref="F14" r:id="rId9"/>
+    <hyperlink ref="F8" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configuration Item List 1.3
</commit_message>
<xml_diff>
--- a/ConfigurationItemList.xlsx
+++ b/ConfigurationItemList.xlsx
@@ -75,9 +75,6 @@
     <t>Defect Tracking System</t>
   </si>
   <si>
-    <t>SoftBugOff.accdb (local file)</t>
-  </si>
-  <si>
     <t>Defects from Test Cases</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>https://github.com/sungori/SoftBugOff/blob/master/UseCases.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/sungori/SoftBugOff/blob/master/SoftBugOff.accdb</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,7 +540,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickBot="1">
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30.75" thickBot="1">
@@ -628,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" thickBot="1">
@@ -648,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" thickBot="1">
@@ -668,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30.75" thickBot="1">
@@ -688,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30.75" thickBot="1">
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30.75" thickBot="1">
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1">
@@ -771,7 +771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1">
+    <row r="12" spans="1:6" ht="30.75" thickBot="1">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -779,16 +779,16 @@
         <v>17</v>
       </c>
       <c r="C12" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="6">
-        <v>41921</v>
+        <v>41928</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>18</v>
+      <c r="F12" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1">
@@ -796,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="7">
         <v>0.1</v>
@@ -816,7 +816,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="7">
         <v>0.6</v>
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30.75" thickBot="1">
@@ -836,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="7">
         <v>1.3</v>
@@ -848,7 +848,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -863,8 +863,9 @@
     <hyperlink ref="F15" r:id="rId8"/>
     <hyperlink ref="F14" r:id="rId9"/>
     <hyperlink ref="F8" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>